<commit_message>
Corrige problemas de carga de dataframes en ejercicios
</commit_message>
<xml_diff>
--- a/inst/tutorials/sesion1/Puestos.xlsx
+++ b/inst/tutorials/sesion1/Puestos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\R\Curso_de_R\Clase_1_Introduccion_R_y_Tidyverse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\R\introR4hr\inst\tutorials\sesion1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{939F474D-2193-4D26-A537-187363858262}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97806EFD-58DE-4805-8260-F6AC204E17D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{D425EF94-2620-4E8A-AEDC-D03C26C636D9}"/>
   </bookViews>

</xml_diff>